<commit_message>
SD-98046 - CCRU - POS KPIs update
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/PoS 2019 - IC HoReCa RestCafeTea.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/PoS 2019 - IC HoReCa RestCafeTea.xlsx
@@ -18,6 +18,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0" vbProcedure="false">'HoReCa Restaurant_Cafe'!$A$1:$AL$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0" vbProcedure="false">'HoReCa Restaurant_Cafe'!$A$1:$AL$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'HoReCa Restaurant_Cafe'!$A$1:$AL$45</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'HoReCa Restaurant_Cafe'!$A$1:$AL$45</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="204">
   <si>
     <t xml:space="preserve">Sorting</t>
   </si>
@@ -477,10 +478,7 @@
     <t xml:space="preserve">Другие активации: Cтекло/Миксабилити</t>
   </si>
   <si>
-    <t xml:space="preserve">Bonaqua, Sprite, Rich, Dobriy, Fanta </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bonaqua, Sprite, Rich, Dobriy, Fanta , SmartWater</t>
+    <t xml:space="preserve">Bonaqua, Sprite, Rich, Dobriy, Fanta, SmartWater, Schweppes</t>
   </si>
   <si>
     <t xml:space="preserve">Mixability, Glass, Mocktails</t>
@@ -925,50 +923,50 @@
   </sheetPr>
   <dimension ref="A1:AL45"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="N32" activeCellId="0" sqref="N32:Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.748987854251"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="35.9919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.3117408906883"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="68.1295546558705"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="68.663967611336"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="32.6720647773279"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="68.663967611336"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="69.3076923076923"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="32.8866396761134"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="39.2064777327935"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="39.2064777327935"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="31.17004048583"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="39.5263157894737"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="39.5263157894737"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="20.995951417004"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="1" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="42.2064777327935"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="28.3846153846154"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="3" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="33.7408906882591"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="42.5263157894737"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="3" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="34.0647773279352"/>
     <col collapsed="false" hidden="false" max="35" min="35" style="1" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="36" min="36" style="1" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="2" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="2" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="38" min="38" style="1" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="1025" min="39" style="1" width="9.10526315789474"/>
   </cols>
@@ -3401,16 +3399,16 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="8" t="s">
+      <c r="N32" s="13" t="s">
         <v>141</v>
       </c>
       <c r="O32" s="7"/>
       <c r="P32" s="7"/>
-      <c r="Q32" s="7" t="s">
+      <c r="Q32" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="R32" s="7" t="s">
         <v>142</v>
-      </c>
-      <c r="R32" s="7" t="s">
-        <v>143</v>
       </c>
       <c r="S32" s="7" t="s">
         <v>53</v>
@@ -3426,7 +3424,7 @@
         <v>117</v>
       </c>
       <c r="Z32" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="AA32" s="7"/>
       <c r="AB32" s="7"/>
@@ -3464,10 +3462,10 @@
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="G33" s="7" t="s">
         <v>145</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>146</v>
       </c>
       <c r="H33" s="7" t="s">
         <v>40</v>
@@ -3524,10 +3522,10 @@
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G34" s="7" t="s">
         <v>147</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>148</v>
       </c>
       <c r="H34" s="7" t="s">
         <v>40</v>
@@ -3585,16 +3583,16 @@
         <v>135</v>
       </c>
       <c r="E35" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="F35" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="G35" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="G35" s="7" t="s">
+      <c r="H35" s="7" t="s">
         <v>151</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>152</v>
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="7" t="n">
@@ -3615,7 +3613,7 @@
       <c r="W35" s="7"/>
       <c r="X35" s="7"/>
       <c r="Y35" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Z35" s="7"/>
       <c r="AA35" s="7"/>
@@ -3637,7 +3635,7 @@
         <v>2</v>
       </c>
       <c r="AK35" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL35" s="7" t="n">
         <v>312</v>
@@ -3657,16 +3655,16 @@
         <v>135</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F36" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G36" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="G36" s="7" t="s">
+      <c r="H36" s="7" t="s">
         <v>156</v>
-      </c>
-      <c r="H36" s="7" t="s">
-        <v>157</v>
       </c>
       <c r="I36" s="7"/>
       <c r="J36" s="7" t="n">
@@ -3684,7 +3682,7 @@
         <v>53</v>
       </c>
       <c r="T36" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="U36" s="7"/>
       <c r="V36" s="7"/>
@@ -3694,7 +3692,7 @@
         <v>55</v>
       </c>
       <c r="Z36" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA36" s="7"/>
       <c r="AB36" s="7"/>
@@ -3731,16 +3729,16 @@
         <v>135</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F37" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="G37" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="G37" s="7" t="s">
+      <c r="H37" s="7" t="s">
         <v>161</v>
-      </c>
-      <c r="H37" s="7" t="s">
-        <v>162</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7" t="n">
@@ -3749,10 +3747,10 @@
       <c r="K37" s="7"/>
       <c r="L37" s="7"/>
       <c r="M37" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="N37" s="8" t="s">
         <v>163</v>
-      </c>
-      <c r="N37" s="8" t="s">
-        <v>164</v>
       </c>
       <c r="O37" s="7"/>
       <c r="P37" s="7"/>
@@ -3762,14 +3760,14 @@
         <v>53</v>
       </c>
       <c r="T37" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="U37" s="7"/>
       <c r="V37" s="7"/>
       <c r="W37" s="7"/>
       <c r="X37" s="7"/>
       <c r="Y37" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Z37" s="7"/>
       <c r="AA37" s="7"/>
@@ -3782,7 +3780,7 @@
       <c r="AF37" s="7"/>
       <c r="AG37" s="7"/>
       <c r="AH37" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AI37" s="7" t="n">
         <v>40</v>
@@ -3809,16 +3807,16 @@
         <v>135</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F38" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G38" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="G38" s="7" t="s">
+      <c r="H38" s="7" t="s">
         <v>168</v>
-      </c>
-      <c r="H38" s="7" t="s">
-        <v>169</v>
       </c>
       <c r="I38" s="7"/>
       <c r="J38" s="7" t="n">
@@ -3827,10 +3825,10 @@
       <c r="K38" s="7"/>
       <c r="L38" s="7"/>
       <c r="M38" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="N38" s="8" t="s">
         <v>163</v>
-      </c>
-      <c r="N38" s="8" t="s">
-        <v>164</v>
       </c>
       <c r="O38" s="7"/>
       <c r="P38" s="7"/>
@@ -3840,14 +3838,14 @@
         <v>53</v>
       </c>
       <c r="T38" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="U38" s="7"/>
       <c r="V38" s="7"/>
       <c r="W38" s="7"/>
       <c r="X38" s="7"/>
       <c r="Y38" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Z38" s="7"/>
       <c r="AA38" s="7"/>
@@ -3860,7 +3858,7 @@
       <c r="AF38" s="7"/>
       <c r="AG38" s="7"/>
       <c r="AH38" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AI38" s="7" t="n">
         <v>41</v>
@@ -3884,22 +3882,22 @@
         <v>39</v>
       </c>
       <c r="D39" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="E39" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="F39" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="G39" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="G39" s="7" t="s">
+      <c r="H39" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="H39" s="7" t="s">
+      <c r="I39" s="7" t="s">
         <v>175</v>
-      </c>
-      <c r="I39" s="7" t="s">
-        <v>176</v>
       </c>
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
@@ -3912,7 +3910,7 @@
       <c r="R39" s="7"/>
       <c r="S39" s="7"/>
       <c r="T39" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="U39" s="7"/>
       <c r="V39" s="7"/>
@@ -3933,7 +3931,7 @@
       </c>
       <c r="AJ39" s="7"/>
       <c r="AK39" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AL39" s="7"/>
     </row>
@@ -3948,31 +3946,31 @@
         <v>39</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>111</v>
       </c>
       <c r="F40" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="G40" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="G40" s="7" t="s">
+      <c r="H40" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="H40" s="7" t="s">
+      <c r="I40" s="7" t="s">
         <v>181</v>
-      </c>
-      <c r="I40" s="7" t="s">
-        <v>182</v>
       </c>
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>
       <c r="M40" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="N40" s="10" t="s">
         <v>183</v>
-      </c>
-      <c r="N40" s="10" t="s">
-        <v>184</v>
       </c>
       <c r="O40" s="7"/>
       <c r="P40" s="7"/>
@@ -3980,7 +3978,7 @@
       <c r="R40" s="7"/>
       <c r="S40" s="7"/>
       <c r="T40" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="U40" s="7"/>
       <c r="V40" s="7"/>
@@ -4016,31 +4014,31 @@
         <v>39</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>119</v>
       </c>
       <c r="F41" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="G41" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="G41" s="7" t="s">
-        <v>186</v>
-      </c>
       <c r="H41" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="I41" s="7" t="s">
         <v>181</v>
-      </c>
-      <c r="I41" s="7" t="s">
-        <v>182</v>
       </c>
       <c r="J41" s="7"/>
       <c r="K41" s="7"/>
       <c r="L41" s="7"/>
       <c r="M41" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N41" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="O41" s="7"/>
       <c r="P41" s="7"/>
@@ -4048,7 +4046,7 @@
       <c r="R41" s="7"/>
       <c r="S41" s="7"/>
       <c r="T41" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="U41" s="7"/>
       <c r="V41" s="7"/>
@@ -4084,31 +4082,31 @@
         <v>39</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>119</v>
       </c>
       <c r="F42" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="G42" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="G42" s="7" t="s">
-        <v>186</v>
-      </c>
       <c r="H42" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="I42" s="7" t="s">
         <v>181</v>
-      </c>
-      <c r="I42" s="7" t="s">
-        <v>182</v>
       </c>
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
       <c r="L42" s="7"/>
       <c r="M42" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N42" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="O42" s="7"/>
       <c r="P42" s="7"/>
@@ -4116,7 +4114,7 @@
       <c r="R42" s="7"/>
       <c r="S42" s="7"/>
       <c r="T42" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="U42" s="7"/>
       <c r="V42" s="7"/>
@@ -4152,31 +4150,31 @@
         <v>39</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E43" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="F43" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="F43" s="7" t="s">
+      <c r="G43" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="G43" s="7" t="s">
-        <v>191</v>
-      </c>
       <c r="H43" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="I43" s="7" t="s">
         <v>181</v>
-      </c>
-      <c r="I43" s="7" t="s">
-        <v>182</v>
       </c>
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
       <c r="L43" s="7"/>
       <c r="M43" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="N43" s="10" t="s">
         <v>192</v>
-      </c>
-      <c r="N43" s="10" t="s">
-        <v>193</v>
       </c>
       <c r="O43" s="7"/>
       <c r="P43" s="7"/>
@@ -4184,7 +4182,7 @@
       <c r="R43" s="7"/>
       <c r="S43" s="7"/>
       <c r="T43" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="U43" s="7"/>
       <c r="V43" s="7"/>
@@ -4205,7 +4203,7 @@
       </c>
       <c r="AJ43" s="7"/>
       <c r="AK43" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AL43" s="7"/>
     </row>
@@ -4220,31 +4218,31 @@
         <v>39</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E44" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="F44" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="F44" s="7" t="s">
+      <c r="G44" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="G44" s="7" t="s">
-        <v>191</v>
-      </c>
       <c r="H44" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="I44" s="7" t="s">
         <v>181</v>
-      </c>
-      <c r="I44" s="7" t="s">
-        <v>182</v>
       </c>
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
       <c r="L44" s="7"/>
       <c r="M44" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N44" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O44" s="7"/>
       <c r="P44" s="7"/>
@@ -4252,7 +4250,7 @@
       <c r="R44" s="7"/>
       <c r="S44" s="7"/>
       <c r="T44" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="U44" s="7"/>
       <c r="V44" s="7"/>
@@ -4273,7 +4271,7 @@
       </c>
       <c r="AJ44" s="7"/>
       <c r="AK44" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AL44" s="7"/>
     </row>
@@ -4288,20 +4286,20 @@
         <v>39</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E45" s="7"/>
       <c r="F45" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="G45" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="G45" s="7" t="s">
+      <c r="H45" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="I45" s="7" t="s">
         <v>197</v>
-      </c>
-      <c r="H45" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="I45" s="7" t="s">
-        <v>198</v>
       </c>
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
@@ -4314,7 +4312,7 @@
       <c r="R45" s="7"/>
       <c r="S45" s="7"/>
       <c r="T45" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="U45" s="7"/>
       <c r="V45" s="7"/>
@@ -4358,7 +4356,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N32:Q32 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4386,10 +4384,10 @@
         <v>12</v>
       </c>
       <c r="G1" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="H1" s="0" t="s">
         <v>199</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>200</v>
       </c>
       <c r="I1" s="0" t="s">
         <v>33</v>
@@ -4398,18 +4396,18 @@
         <v>30</v>
       </c>
       <c r="K1" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="L1" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="M1" s="0" t="s">
         <v>202</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PROS-11596 - CCRU - POS KPIs fix
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/PoS 2019 - IC HoReCa RestCafeTea.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/PoS 2019 - IC HoReCa RestCafeTea.xlsx
@@ -478,7 +478,7 @@
     <t xml:space="preserve">Другие активации: Cтекло/Миксабилити</t>
   </si>
   <si>
-    <t xml:space="preserve">Bonaqua, Sprite, Rich, Dobriy, Fanta, SmartWater, Schweppes</t>
+    <t xml:space="preserve">Bonaqua, Sprite, Rich, Dobriy, Fanta, SmartWater</t>
   </si>
   <si>
     <t xml:space="preserve">Mixability, Glass, Mocktails</t>
@@ -720,7 +720,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -737,6 +737,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFFCC00"/>
       </patternFill>
     </fill>
   </fills>
@@ -783,7 +789,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -837,6 +843,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -923,10 +933,10 @@
   </sheetPr>
   <dimension ref="A1:AL45"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="N32" activeCellId="0" sqref="N32:Q32"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="R35" activeCellId="0" sqref="R35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -943,10 +953,10 @@
     <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.1740890688259"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="1" width="39.5263157894737"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="39.5263157894737"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="55.7570850202429"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="1" width="22.1740890688259"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="1" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="55.7570850202429"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="1" width="26.3522267206478"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="1" width="20.995951417004"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="1" width="14.0323886639676"/>
@@ -3399,12 +3409,12 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="13" t="s">
+      <c r="N32" s="14" t="s">
         <v>141</v>
       </c>
       <c r="O32" s="7"/>
       <c r="P32" s="7"/>
-      <c r="Q32" s="13" t="s">
+      <c r="Q32" s="14" t="s">
         <v>141</v>
       </c>
       <c r="R32" s="7" t="s">
@@ -4356,7 +4366,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="N32:Q32 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>